<commit_message>
PROS-11537 - CCRU - Unit Tests - Development
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Tests/Data/test_case_data.xlsx
+++ b/Projects/CCRU/Tests/Data/test_case_data.xlsx
@@ -14,6 +14,9 @@
     <sheet name="store_areas" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="scif" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$Z$35</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="92">
   <si>
     <t xml:space="preserve">product_fk</t>
   </si>
@@ -281,10 +284,25 @@
     <t xml:space="preserve">facings</t>
   </si>
   <si>
+    <t xml:space="preserve">1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">200</t>
+    <t xml:space="preserve">0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">104</t>
   </si>
 </sst>
 </file>
@@ -396,6 +414,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -1262,7 +1284,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -1529,13 +1551,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T51" activeCellId="0" sqref="T51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1646,7 +1668,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -1740,7 +1762,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -1834,7 +1856,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -1928,7 +1950,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -2210,7 +2232,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>5</v>
       </c>
@@ -2304,7 +2326,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>5</v>
       </c>
@@ -2398,7 +2420,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>5</v>
       </c>
@@ -2586,7 +2608,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>6</v>
       </c>
@@ -2671,7 +2693,7 @@
         <v>65</v>
       </c>
       <c r="X12" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y12" s="0" t="s">
         <v>86</v>
@@ -2680,7 +2702,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>7</v>
       </c>
@@ -2765,7 +2787,7 @@
         <v>65</v>
       </c>
       <c r="X13" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y13" s="0" t="s">
         <v>86</v>
@@ -2859,7 +2881,7 @@
         <v>65</v>
       </c>
       <c r="X14" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y14" s="0" t="s">
         <v>86</v>
@@ -2953,7 +2975,7 @@
         <v>65</v>
       </c>
       <c r="X15" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y15" s="0" t="s">
         <v>86</v>
@@ -2962,7 +2984,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>7</v>
       </c>
@@ -3047,7 +3069,7 @@
         <v>65</v>
       </c>
       <c r="X16" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y16" s="0" t="s">
         <v>86</v>
@@ -3056,7 +3078,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>7</v>
       </c>
@@ -3141,7 +3163,7 @@
         <v>65</v>
       </c>
       <c r="X17" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y17" s="0" t="s">
         <v>86</v>
@@ -3150,7 +3172,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>7</v>
       </c>
@@ -3235,7 +3257,7 @@
         <v>65</v>
       </c>
       <c r="X18" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y18" s="0" t="s">
         <v>86</v>
@@ -3244,7 +3266,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>7</v>
       </c>
@@ -3329,7 +3351,7 @@
         <v>65</v>
       </c>
       <c r="X19" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y19" s="0" t="s">
         <v>86</v>
@@ -3338,7 +3360,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>7</v>
       </c>
@@ -3423,7 +3445,7 @@
         <v>65</v>
       </c>
       <c r="X20" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y20" s="0" t="s">
         <v>86</v>
@@ -3432,7 +3454,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>7</v>
       </c>
@@ -3517,7 +3539,7 @@
         <v>65</v>
       </c>
       <c r="X21" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y21" s="0" t="s">
         <v>86</v>
@@ -3526,7 +3548,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>8</v>
       </c>
@@ -3611,7 +3633,7 @@
         <v>65</v>
       </c>
       <c r="X22" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y22" s="0" t="s">
         <v>86</v>
@@ -3620,7 +3642,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>9</v>
       </c>
@@ -3705,7 +3727,7 @@
         <v>65</v>
       </c>
       <c r="X23" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y23" s="0" t="s">
         <v>86</v>
@@ -3799,7 +3821,7 @@
         <v>65</v>
       </c>
       <c r="X24" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y24" s="0" t="s">
         <v>86</v>
@@ -3893,7 +3915,7 @@
         <v>65</v>
       </c>
       <c r="X25" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y25" s="0" t="s">
         <v>86</v>
@@ -3902,7 +3924,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>10</v>
       </c>
@@ -3987,7 +4009,7 @@
         <v>65</v>
       </c>
       <c r="X26" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y26" s="0" t="s">
         <v>86</v>
@@ -3996,7 +4018,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>10</v>
       </c>
@@ -4081,7 +4103,7 @@
         <v>65</v>
       </c>
       <c r="X27" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y27" s="0" t="s">
         <v>86</v>
@@ -4090,7 +4112,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>10</v>
       </c>
@@ -4175,7 +4197,7 @@
         <v>65</v>
       </c>
       <c r="X28" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y28" s="0" t="s">
         <v>86</v>
@@ -4184,7 +4206,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>10</v>
       </c>
@@ -4269,7 +4291,7 @@
         <v>65</v>
       </c>
       <c r="X29" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y29" s="0" t="s">
         <v>86</v>
@@ -4278,7 +4300,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>10</v>
       </c>
@@ -4363,7 +4385,7 @@
         <v>65</v>
       </c>
       <c r="X30" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Y30" s="0" t="s">
         <v>86</v>
@@ -4372,7 +4394,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>11</v>
       </c>
@@ -4457,16 +4479,16 @@
         <v>66</v>
       </c>
       <c r="X31" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="Y31" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="Z31" s="0" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>12</v>
       </c>
@@ -4551,16 +4573,16 @@
         <v>66</v>
       </c>
       <c r="X32" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="Y32" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="Z32" s="0" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>13</v>
       </c>
@@ -4645,16 +4667,16 @@
         <v>66</v>
       </c>
       <c r="X33" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="Y33" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="Z33" s="0" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>14</v>
       </c>
@@ -4739,16 +4761,16 @@
         <v>68</v>
       </c>
       <c r="X34" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Y34" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="Z34" s="0" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>15</v>
       </c>
@@ -4833,16 +4855,35 @@
         <v>68</v>
       </c>
       <c r="X35" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Y35" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="Z35" s="0" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Z35">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="Brand_21"/>
+        <filter val="Brand_12"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="16">
+      <filters>
+        <filter val="SubCat_32"/>
+        <filter val="SubCat_13"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="25">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Loc_1"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4850,5 +4891,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
availability test debugged + sos test developed and debugged
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Tests/Data/test_case_data.xlsx
+++ b/Projects/CCRU/Tests/Data/test_case_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,6 +20,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">scif!$A$1:$Z$35</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">scif!$A$1:$Z$35</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">scif!$A$1:$Z$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">scif!$A$1:$Z$35</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -435,22 +436,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6518218623482"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3684210526316"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6518218623482"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.5384615384615"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8542510121457"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7408906882591"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.3967611336032"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1983805668016"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.4251012145749"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.1093117408907"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.0526315789474"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="5.48582995951417"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0526315789474"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9676113360324"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6558704453441"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.8825910931174"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.251012145749"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.5384615384615"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.9109311740891"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.2550607287449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.9676113360324"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="5.82591093117409"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.6558704453441"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,16 +1288,17 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3967611336032"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3967611336032"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="25.8218623481781"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1093117408907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5384615384615"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7651821862348"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="27.6518218623482"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2550607287449"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1407,9 +1410,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3967611336032"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1133603238866"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6558704453441"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5384615384615"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0242914979757"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1502,8 +1506,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.080971659919"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.2226720647773"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,40 +1556,41 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H47" activeCellId="0" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4534412955466"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5101214574899"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3967611336032"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1133603238866"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6518218623482"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.3684210526316"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.995951417004"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.7408906882591"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.5384615384615"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.3967611336032"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.1983805668016"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.1417004048583"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.1093117408907"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.0526315789474"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="5.48582995951417"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="10.8542510121457"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.3967611336032"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="25.8218623481781"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.1093117408907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.22672064777328"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3684210526316"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3117408906883"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6558704453441"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5384615384615"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.0242914979757"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.1376518218623"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.9676113360324"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.8825910931174"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.251012145749"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5384615384615"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0526315789474"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.2550607287449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.9676113360324"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="5.82591093117409"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="11.6558704453441"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="21.251012145749"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.7651821862348"/>
+    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="27.6518218623482"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.2550607287449"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2513,7 +2519,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>5</v>
       </c>
@@ -4675,7 +4681,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>14</v>
       </c>
@@ -4769,7 +4775,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>15</v>
       </c>
@@ -4864,7 +4870,21 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z35"/>
+  <autoFilter ref="A1:Z35">
+    <filterColumn colId="14">
+      <filters>
+        <filter val="Cat_2"/>
+        <filter val="Cat_1"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="22">
+      <filters>
+        <filter val="Scene_type_3"/>
+        <filter val="Scene_type_2"/>
+        <filter val="Scene_type_1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
share of CCH doors developed and debugged
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Tests/Data/test_case_data.xlsx
+++ b/Projects/CCRU/Tests/Data/test_case_data.xlsx
@@ -15,12 +15,12 @@
     <sheet name="scif" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$Z$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$Z$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">scif!$A$1:$Z$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">scif!$A$1:$Z$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">scif!$A$1:$Z$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">scif!$A$1:$Z$35</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$Z$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$Z$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">scif!$A$1:$Z$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">scif!$A$1:$Z$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">scif!$A$1:$Z$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">scif!$A$1:$Z$36</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="92">
   <si>
     <t xml:space="preserve">product_fk</t>
   </si>
@@ -289,13 +289,13 @@
     <t xml:space="preserve">facings</t>
   </si>
   <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">0.5</t>
@@ -430,8 +430,8 @@
   </sheetPr>
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -601,7 +601,7 @@
         <v>23</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="P3" s="0" t="s">
         <v>24</v>
@@ -703,7 +703,7 @@
         <v>23</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>1.5</v>
+        <v>0.9</v>
       </c>
       <c r="P5" s="0" t="s">
         <v>24</v>
@@ -1060,7 +1060,7 @@
         <v>23</v>
       </c>
       <c r="O12" s="0" t="n">
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="P12" s="0" t="s">
         <v>24</v>
@@ -1556,13 +1556,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z35"/>
+  <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H47" activeCellId="0" sqref="H47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q13" activeCellId="0" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1834,7 +1834,7 @@
       </c>
       <c r="S3" s="0" t="n">
         <f aca="false">VLOOKUP($D3,products!$A$2:$P$16,15,0)</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="T3" s="0" t="str">
         <f aca="false">VLOOKUP($D3,products!$A$2:$P$16,16,0)</f>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="S5" s="0" t="n">
         <f aca="false">VLOOKUP($D5,products!$A$2:$P$16,15,0)</f>
-        <v>1.5</v>
+        <v>0.9</v>
       </c>
       <c r="T5" s="0" t="str">
         <f aca="false">VLOOKUP($D5,products!$A$2:$P$16,16,0)</f>
@@ -2145,7 +2145,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
@@ -2333,7 +2333,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -2519,9 +2519,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -2533,7 +2533,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>1</v>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
@@ -2709,7 +2709,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1</v>
@@ -2774,7 +2774,7 @@
       </c>
       <c r="S13" s="0" t="n">
         <f aca="false">VLOOKUP($D13,products!$A$2:$P$16,15,0)</f>
-        <v>1.5</v>
+        <v>0.9</v>
       </c>
       <c r="T13" s="0" t="str">
         <f aca="false">VLOOKUP($D13,products!$A$2:$P$16,16,0)</f>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -2897,7 +2897,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -2991,7 +2991,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
@@ -3085,7 +3085,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
@@ -3179,7 +3179,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
@@ -3273,7 +3273,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
@@ -3367,7 +3367,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
@@ -3432,7 +3432,7 @@
       </c>
       <c r="S20" s="0" t="n">
         <f aca="false">VLOOKUP($D20,products!$A$2:$P$16,15,0)</f>
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="T20" s="0" t="str">
         <f aca="false">VLOOKUP($D20,products!$A$2:$P$16,16,0)</f>
@@ -3461,7 +3461,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
@@ -3473,7 +3473,7 @@
         <v>12</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>2</v>
@@ -3555,36 +3555,36 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I22" s="0" t="str">
         <f aca="false">VLOOKUP(D22,products!$A$2:$P$16,2,0)</f>
-        <v>Product_111_11_01</v>
+        <v>Product_211_32_15</v>
       </c>
       <c r="J22" s="0" t="str">
         <f aca="false">VLOOKUP(D22,products!$A$2:$P$16,3,0)</f>
-        <v>111_11_01</v>
+        <v>211_32_15</v>
       </c>
       <c r="K22" s="0" t="str">
         <f aca="false">VLOOKUP(D22,products!$A$2:$P$16,4,0)</f>
@@ -3592,11 +3592,11 @@
       </c>
       <c r="L22" s="0" t="str">
         <f aca="false">VLOOKUP($D22,products!$A$2:$P$16,8,0)</f>
-        <v>Brand_11</v>
+        <v>Brand_21</v>
       </c>
       <c r="M22" s="0" t="str">
         <f aca="false">VLOOKUP($D22,products!$A$2:$P$16,6,0)</f>
-        <v>TCCC</v>
+        <v>Man_2</v>
       </c>
       <c r="N22" s="0" t="n">
         <f aca="false">VLOOKUP($D22,products!$A$2:$P$16,10,0)</f>
@@ -3604,23 +3604,23 @@
       </c>
       <c r="O22" s="0" t="str">
         <f aca="false">VLOOKUP($D22,products!$A$2:$P$16,11,0)</f>
-        <v>Cat_1</v>
+        <v>Cat_3</v>
       </c>
       <c r="P22" s="0" t="n">
         <f aca="false">D22</f>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="Q22" s="0" t="str">
         <f aca="false">VLOOKUP($D22,products!$A$2:$P$16,13,0)</f>
-        <v>SubCat_11</v>
+        <v>SubCat_32</v>
       </c>
       <c r="R22" s="0" t="str">
         <f aca="false">VLOOKUP($D22,products!$A$2:$P$16,14,0)</f>
-        <v>FF_1</v>
+        <v>FF_3</v>
       </c>
       <c r="S22" s="0" t="n">
         <f aca="false">VLOOKUP($D22,products!$A$2:$P$16,15,0)</f>
-        <v>0.5</v>
+        <v>0.33</v>
       </c>
       <c r="T22" s="0" t="str">
         <f aca="false">VLOOKUP($D22,products!$A$2:$P$16,16,0)</f>
@@ -3628,11 +3628,11 @@
       </c>
       <c r="U22" s="0" t="str">
         <f aca="false">VLOOKUP($D22,products!$A$2:$P$16,8,0)</f>
-        <v>Brand_11</v>
+        <v>Brand_21</v>
       </c>
       <c r="V22" s="0" t="str">
         <f aca="false">VLOOKUP($D22,products!$A$2:$P$16,9,0)</f>
-        <v>SubBrand_111</v>
+        <v>SubBrand_211</v>
       </c>
       <c r="W22" s="0" t="s">
         <v>65</v>
@@ -3649,7 +3649,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>
@@ -3658,10 +3658,10 @@
         <v>3</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>3</v>
@@ -3674,11 +3674,11 @@
       </c>
       <c r="I23" s="0" t="str">
         <f aca="false">VLOOKUP(D23,products!$A$2:$P$16,2,0)</f>
-        <v>Product_111_11_02</v>
+        <v>Product_111_11_01</v>
       </c>
       <c r="J23" s="0" t="str">
         <f aca="false">VLOOKUP(D23,products!$A$2:$P$16,3,0)</f>
-        <v>111_11_02</v>
+        <v>111_11_01</v>
       </c>
       <c r="K23" s="0" t="str">
         <f aca="false">VLOOKUP(D23,products!$A$2:$P$16,4,0)</f>
@@ -3702,7 +3702,7 @@
       </c>
       <c r="P23" s="0" t="n">
         <f aca="false">D23</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q23" s="0" t="str">
         <f aca="false">VLOOKUP($D23,products!$A$2:$P$16,13,0)</f>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="S23" s="0" t="n">
         <f aca="false">VLOOKUP($D23,products!$A$2:$P$16,15,0)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="T23" s="0" t="str">
         <f aca="false">VLOOKUP($D23,products!$A$2:$P$16,16,0)</f>
@@ -3743,7 +3743,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1</v>
@@ -3752,10 +3752,10 @@
         <v>3</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>3</v>
@@ -3768,11 +3768,11 @@
       </c>
       <c r="I24" s="0" t="str">
         <f aca="false">VLOOKUP(D24,products!$A$2:$P$16,2,0)</f>
-        <v>Product_121_13_05</v>
+        <v>Product_111_11_02</v>
       </c>
       <c r="J24" s="0" t="str">
         <f aca="false">VLOOKUP(D24,products!$A$2:$P$16,3,0)</f>
-        <v>121_13_05</v>
+        <v>111_11_02</v>
       </c>
       <c r="K24" s="0" t="str">
         <f aca="false">VLOOKUP(D24,products!$A$2:$P$16,4,0)</f>
@@ -3780,7 +3780,7 @@
       </c>
       <c r="L24" s="0" t="str">
         <f aca="false">VLOOKUP($D24,products!$A$2:$P$16,8,0)</f>
-        <v>Brand_12</v>
+        <v>Brand_11</v>
       </c>
       <c r="M24" s="0" t="str">
         <f aca="false">VLOOKUP($D24,products!$A$2:$P$16,6,0)</f>
@@ -3796,11 +3796,11 @@
       </c>
       <c r="P24" s="0" t="n">
         <f aca="false">D24</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q24" s="0" t="str">
         <f aca="false">VLOOKUP($D24,products!$A$2:$P$16,13,0)</f>
-        <v>SubCat_13</v>
+        <v>SubCat_11</v>
       </c>
       <c r="R24" s="0" t="str">
         <f aca="false">VLOOKUP($D24,products!$A$2:$P$16,14,0)</f>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="S24" s="0" t="n">
         <f aca="false">VLOOKUP($D24,products!$A$2:$P$16,15,0)</f>
-        <v>0.5</v>
+        <v>0.33</v>
       </c>
       <c r="T24" s="0" t="str">
         <f aca="false">VLOOKUP($D24,products!$A$2:$P$16,16,0)</f>
@@ -3816,11 +3816,11 @@
       </c>
       <c r="U24" s="0" t="str">
         <f aca="false">VLOOKUP($D24,products!$A$2:$P$16,8,0)</f>
-        <v>Brand_12</v>
+        <v>Brand_11</v>
       </c>
       <c r="V24" s="0" t="str">
         <f aca="false">VLOOKUP($D24,products!$A$2:$P$16,9,0)</f>
-        <v>SubBrand_121</v>
+        <v>SubBrand_111</v>
       </c>
       <c r="W24" s="0" t="s">
         <v>65</v>
@@ -3837,7 +3837,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>1</v>
@@ -3846,10 +3846,10 @@
         <v>3</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>3</v>
@@ -3862,11 +3862,11 @@
       </c>
       <c r="I25" s="0" t="str">
         <f aca="false">VLOOKUP(D25,products!$A$2:$P$16,2,0)</f>
-        <v>Product_121_13_06</v>
+        <v>Product_121_13_05</v>
       </c>
       <c r="J25" s="0" t="str">
         <f aca="false">VLOOKUP(D25,products!$A$2:$P$16,3,0)</f>
-        <v>121_13_06</v>
+        <v>121_13_05</v>
       </c>
       <c r="K25" s="0" t="str">
         <f aca="false">VLOOKUP(D25,products!$A$2:$P$16,4,0)</f>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P25" s="0" t="n">
         <f aca="false">D25</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q25" s="0" t="str">
         <f aca="false">VLOOKUP($D25,products!$A$2:$P$16,13,0)</f>
@@ -3931,7 +3931,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1</v>
@@ -3940,10 +3940,10 @@
         <v>3</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>3</v>
@@ -3956,11 +3956,11 @@
       </c>
       <c r="I26" s="0" t="str">
         <f aca="false">VLOOKUP(D26,products!$A$2:$P$16,2,0)</f>
-        <v>Product_121_21_07</v>
+        <v>Product_121_13_06</v>
       </c>
       <c r="J26" s="0" t="str">
         <f aca="false">VLOOKUP(D26,products!$A$2:$P$16,3,0)</f>
-        <v>121_21_07</v>
+        <v>121_13_06</v>
       </c>
       <c r="K26" s="0" t="str">
         <f aca="false">VLOOKUP(D26,products!$A$2:$P$16,4,0)</f>
@@ -3980,23 +3980,23 @@
       </c>
       <c r="O26" s="0" t="str">
         <f aca="false">VLOOKUP($D26,products!$A$2:$P$16,11,0)</f>
-        <v>Cat_2</v>
+        <v>Cat_1</v>
       </c>
       <c r="P26" s="0" t="n">
         <f aca="false">D26</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q26" s="0" t="str">
         <f aca="false">VLOOKUP($D26,products!$A$2:$P$16,13,0)</f>
-        <v>SubCat_21</v>
+        <v>SubCat_13</v>
       </c>
       <c r="R26" s="0" t="str">
         <f aca="false">VLOOKUP($D26,products!$A$2:$P$16,14,0)</f>
-        <v>FF_2</v>
+        <v>FF_1</v>
       </c>
       <c r="S26" s="0" t="n">
         <f aca="false">VLOOKUP($D26,products!$A$2:$P$16,15,0)</f>
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T26" s="0" t="str">
         <f aca="false">VLOOKUP($D26,products!$A$2:$P$16,16,0)</f>
@@ -4025,7 +4025,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1</v>
@@ -4034,10 +4034,10 @@
         <v>3</v>
       </c>
       <c r="D27" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E27" s="0" t="n">
         <v>8</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>12</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>3</v>
@@ -4050,11 +4050,11 @@
       </c>
       <c r="I27" s="0" t="str">
         <f aca="false">VLOOKUP(D27,products!$A$2:$P$16,2,0)</f>
-        <v>Product_122_21_08</v>
+        <v>Product_121_21_07</v>
       </c>
       <c r="J27" s="0" t="str">
         <f aca="false">VLOOKUP(D27,products!$A$2:$P$16,3,0)</f>
-        <v>122_21_08</v>
+        <v>121_21_07</v>
       </c>
       <c r="K27" s="0" t="str">
         <f aca="false">VLOOKUP(D27,products!$A$2:$P$16,4,0)</f>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="P27" s="0" t="n">
         <f aca="false">D27</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q27" s="0" t="str">
         <f aca="false">VLOOKUP($D27,products!$A$2:$P$16,13,0)</f>
@@ -4086,11 +4086,11 @@
       </c>
       <c r="R27" s="0" t="str">
         <f aca="false">VLOOKUP($D27,products!$A$2:$P$16,14,0)</f>
-        <v>FF_1</v>
+        <v>FF_2</v>
       </c>
       <c r="S27" s="0" t="n">
         <f aca="false">VLOOKUP($D27,products!$A$2:$P$16,15,0)</f>
-        <v>0.5</v>
+        <v>0.33</v>
       </c>
       <c r="T27" s="0" t="str">
         <f aca="false">VLOOKUP($D27,products!$A$2:$P$16,16,0)</f>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="V27" s="0" t="str">
         <f aca="false">VLOOKUP($D27,products!$A$2:$P$16,9,0)</f>
-        <v>SubBrand_122</v>
+        <v>SubBrand_121</v>
       </c>
       <c r="W27" s="0" t="s">
         <v>65</v>
@@ -4119,7 +4119,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1</v>
@@ -4128,10 +4128,10 @@
         <v>3</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>3</v>
@@ -4144,11 +4144,11 @@
       </c>
       <c r="I28" s="0" t="str">
         <f aca="false">VLOOKUP(D28,products!$A$2:$P$16,2,0)</f>
-        <v>Product_122_22_09</v>
+        <v>Product_122_21_08</v>
       </c>
       <c r="J28" s="0" t="str">
         <f aca="false">VLOOKUP(D28,products!$A$2:$P$16,3,0)</f>
-        <v>122_22_09</v>
+        <v>122_21_08</v>
       </c>
       <c r="K28" s="0" t="str">
         <f aca="false">VLOOKUP(D28,products!$A$2:$P$16,4,0)</f>
@@ -4172,11 +4172,11 @@
       </c>
       <c r="P28" s="0" t="n">
         <f aca="false">D28</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q28" s="0" t="str">
         <f aca="false">VLOOKUP($D28,products!$A$2:$P$16,13,0)</f>
-        <v>SubCat_22</v>
+        <v>SubCat_21</v>
       </c>
       <c r="R28" s="0" t="str">
         <f aca="false">VLOOKUP($D28,products!$A$2:$P$16,14,0)</f>
@@ -4213,7 +4213,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1</v>
@@ -4222,10 +4222,10 @@
         <v>3</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>3</v>
@@ -4238,11 +4238,11 @@
       </c>
       <c r="I29" s="0" t="str">
         <f aca="false">VLOOKUP(D29,products!$A$2:$P$16,2,0)</f>
-        <v>Product_122_22_10</v>
+        <v>Product_122_22_09</v>
       </c>
       <c r="J29" s="0" t="str">
         <f aca="false">VLOOKUP(D29,products!$A$2:$P$16,3,0)</f>
-        <v>122_22_10</v>
+        <v>122_22_09</v>
       </c>
       <c r="K29" s="0" t="str">
         <f aca="false">VLOOKUP(D29,products!$A$2:$P$16,4,0)</f>
@@ -4266,7 +4266,7 @@
       </c>
       <c r="P29" s="0" t="n">
         <f aca="false">D29</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q29" s="0" t="str">
         <f aca="false">VLOOKUP($D29,products!$A$2:$P$16,13,0)</f>
@@ -4274,11 +4274,11 @@
       </c>
       <c r="R29" s="0" t="str">
         <f aca="false">VLOOKUP($D29,products!$A$2:$P$16,14,0)</f>
-        <v>FF_3</v>
+        <v>FF_1</v>
       </c>
       <c r="S29" s="0" t="n">
         <f aca="false">VLOOKUP($D29,products!$A$2:$P$16,15,0)</f>
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T29" s="0" t="str">
         <f aca="false">VLOOKUP($D29,products!$A$2:$P$16,16,0)</f>
@@ -4307,7 +4307,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -4316,10 +4316,10 @@
         <v>3</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>3</v>
@@ -4332,11 +4332,11 @@
       </c>
       <c r="I30" s="0" t="str">
         <f aca="false">VLOOKUP(D30,products!$A$2:$P$16,2,0)</f>
-        <v>Product_113_23_11</v>
+        <v>Product_122_22_10</v>
       </c>
       <c r="J30" s="0" t="str">
         <f aca="false">VLOOKUP(D30,products!$A$2:$P$16,3,0)</f>
-        <v>113_23_11</v>
+        <v>122_22_10</v>
       </c>
       <c r="K30" s="0" t="str">
         <f aca="false">VLOOKUP(D30,products!$A$2:$P$16,4,0)</f>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="L30" s="0" t="str">
         <f aca="false">VLOOKUP($D30,products!$A$2:$P$16,8,0)</f>
-        <v>Brand_11</v>
+        <v>Brand_12</v>
       </c>
       <c r="M30" s="0" t="str">
         <f aca="false">VLOOKUP($D30,products!$A$2:$P$16,6,0)</f>
@@ -4360,19 +4360,19 @@
       </c>
       <c r="P30" s="0" t="n">
         <f aca="false">D30</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q30" s="0" t="str">
         <f aca="false">VLOOKUP($D30,products!$A$2:$P$16,13,0)</f>
-        <v>SubCat_23</v>
+        <v>SubCat_22</v>
       </c>
       <c r="R30" s="0" t="str">
         <f aca="false">VLOOKUP($D30,products!$A$2:$P$16,14,0)</f>
-        <v>FF_1</v>
+        <v>FF_3</v>
       </c>
       <c r="S30" s="0" t="n">
         <f aca="false">VLOOKUP($D30,products!$A$2:$P$16,15,0)</f>
-        <v>2</v>
+        <v>0.33</v>
       </c>
       <c r="T30" s="0" t="str">
         <f aca="false">VLOOKUP($D30,products!$A$2:$P$16,16,0)</f>
@@ -4380,11 +4380,11 @@
       </c>
       <c r="U30" s="0" t="str">
         <f aca="false">VLOOKUP($D30,products!$A$2:$P$16,8,0)</f>
-        <v>Brand_11</v>
+        <v>Brand_12</v>
       </c>
       <c r="V30" s="0" t="str">
         <f aca="false">VLOOKUP($D30,products!$A$2:$P$16,9,0)</f>
-        <v>SubBrand_113</v>
+        <v>SubBrand_122</v>
       </c>
       <c r="W30" s="0" t="s">
         <v>65</v>
@@ -4401,36 +4401,36 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D31" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D31" s="0" t="n">
+      <c r="E31" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F31" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E31" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="F31" s="0" t="n">
-        <v>4</v>
-      </c>
       <c r="G31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I31" s="0" t="str">
         <f aca="false">VLOOKUP(D31,products!$A$2:$P$16,2,0)</f>
-        <v>Product_112_12_03</v>
+        <v>Product_113_23_11</v>
       </c>
       <c r="J31" s="0" t="str">
         <f aca="false">VLOOKUP(D31,products!$A$2:$P$16,3,0)</f>
-        <v>112_12_03</v>
+        <v>113_23_11</v>
       </c>
       <c r="K31" s="0" t="str">
         <f aca="false">VLOOKUP(D31,products!$A$2:$P$16,4,0)</f>
@@ -4450,23 +4450,23 @@
       </c>
       <c r="O31" s="0" t="str">
         <f aca="false">VLOOKUP($D31,products!$A$2:$P$16,11,0)</f>
-        <v>Cat_1</v>
+        <v>Cat_2</v>
       </c>
       <c r="P31" s="0" t="n">
         <f aca="false">D31</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="Q31" s="0" t="str">
         <f aca="false">VLOOKUP($D31,products!$A$2:$P$16,13,0)</f>
-        <v>SubCat_12</v>
+        <v>SubCat_23</v>
       </c>
       <c r="R31" s="0" t="str">
         <f aca="false">VLOOKUP($D31,products!$A$2:$P$16,14,0)</f>
-        <v>FF_2</v>
+        <v>FF_1</v>
       </c>
       <c r="S31" s="0" t="n">
         <f aca="false">VLOOKUP($D31,products!$A$2:$P$16,15,0)</f>
-        <v>0.33</v>
+        <v>0.9</v>
       </c>
       <c r="T31" s="0" t="str">
         <f aca="false">VLOOKUP($D31,products!$A$2:$P$16,16,0)</f>
@@ -4478,24 +4478,24 @@
       </c>
       <c r="V31" s="0" t="str">
         <f aca="false">VLOOKUP($D31,products!$A$2:$P$16,9,0)</f>
-        <v>SubBrand_112</v>
+        <v>SubBrand_113</v>
       </c>
       <c r="W31" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="X31" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Y31" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="Z31" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -4504,10 +4504,10 @@
         <v>4</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>4</v>
@@ -4520,11 +4520,11 @@
       </c>
       <c r="I32" s="0" t="str">
         <f aca="false">VLOOKUP(D32,products!$A$2:$P$16,2,0)</f>
-        <v>Product_112_12_04</v>
+        <v>Product_112_12_03</v>
       </c>
       <c r="J32" s="0" t="str">
         <f aca="false">VLOOKUP(D32,products!$A$2:$P$16,3,0)</f>
-        <v>112_12_04</v>
+        <v>112_12_03</v>
       </c>
       <c r="K32" s="0" t="str">
         <f aca="false">VLOOKUP(D32,products!$A$2:$P$16,4,0)</f>
@@ -4548,7 +4548,7 @@
       </c>
       <c r="P32" s="0" t="n">
         <f aca="false">D32</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q32" s="0" t="str">
         <f aca="false">VLOOKUP($D32,products!$A$2:$P$16,13,0)</f>
@@ -4556,11 +4556,11 @@
       </c>
       <c r="R32" s="0" t="str">
         <f aca="false">VLOOKUP($D32,products!$A$2:$P$16,14,0)</f>
-        <v>FF_1</v>
+        <v>FF_2</v>
       </c>
       <c r="S32" s="0" t="n">
         <f aca="false">VLOOKUP($D32,products!$A$2:$P$16,15,0)</f>
-        <v>1.5</v>
+        <v>0.33</v>
       </c>
       <c r="T32" s="0" t="str">
         <f aca="false">VLOOKUP($D32,products!$A$2:$P$16,16,0)</f>
@@ -4589,7 +4589,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
@@ -4598,10 +4598,10 @@
         <v>4</v>
       </c>
       <c r="D33" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E33" s="0" t="n">
         <v>5</v>
-      </c>
-      <c r="E33" s="0" t="n">
-        <v>4</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>4</v>
@@ -4614,11 +4614,11 @@
       </c>
       <c r="I33" s="0" t="str">
         <f aca="false">VLOOKUP(D33,products!$A$2:$P$16,2,0)</f>
-        <v>Product_121_13_05</v>
+        <v>Product_112_12_04</v>
       </c>
       <c r="J33" s="0" t="str">
         <f aca="false">VLOOKUP(D33,products!$A$2:$P$16,3,0)</f>
-        <v>121_13_05</v>
+        <v>112_12_04</v>
       </c>
       <c r="K33" s="0" t="str">
         <f aca="false">VLOOKUP(D33,products!$A$2:$P$16,4,0)</f>
@@ -4626,7 +4626,7 @@
       </c>
       <c r="L33" s="0" t="str">
         <f aca="false">VLOOKUP($D33,products!$A$2:$P$16,8,0)</f>
-        <v>Brand_12</v>
+        <v>Brand_11</v>
       </c>
       <c r="M33" s="0" t="str">
         <f aca="false">VLOOKUP($D33,products!$A$2:$P$16,6,0)</f>
@@ -4642,11 +4642,11 @@
       </c>
       <c r="P33" s="0" t="n">
         <f aca="false">D33</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q33" s="0" t="str">
         <f aca="false">VLOOKUP($D33,products!$A$2:$P$16,13,0)</f>
-        <v>SubCat_13</v>
+        <v>SubCat_12</v>
       </c>
       <c r="R33" s="0" t="str">
         <f aca="false">VLOOKUP($D33,products!$A$2:$P$16,14,0)</f>
@@ -4654,7 +4654,7 @@
       </c>
       <c r="S33" s="0" t="n">
         <f aca="false">VLOOKUP($D33,products!$A$2:$P$16,15,0)</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="T33" s="0" t="str">
         <f aca="false">VLOOKUP($D33,products!$A$2:$P$16,16,0)</f>
@@ -4662,11 +4662,11 @@
       </c>
       <c r="U33" s="0" t="str">
         <f aca="false">VLOOKUP($D33,products!$A$2:$P$16,8,0)</f>
-        <v>Brand_12</v>
+        <v>Brand_11</v>
       </c>
       <c r="V33" s="0" t="str">
         <f aca="false">VLOOKUP($D33,products!$A$2:$P$16,9,0)</f>
-        <v>SubBrand_121</v>
+        <v>SubBrand_112</v>
       </c>
       <c r="W33" s="0" t="s">
         <v>66</v>
@@ -4681,38 +4681,38 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C34" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D34" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D34" s="0" t="n">
-        <v>8</v>
-      </c>
       <c r="E34" s="0" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I34" s="0" t="str">
         <f aca="false">VLOOKUP(D34,products!$A$2:$P$16,2,0)</f>
-        <v>Product_122_21_08</v>
+        <v>Product_121_13_05</v>
       </c>
       <c r="J34" s="0" t="str">
         <f aca="false">VLOOKUP(D34,products!$A$2:$P$16,3,0)</f>
-        <v>122_21_08</v>
+        <v>121_13_05</v>
       </c>
       <c r="K34" s="0" t="str">
         <f aca="false">VLOOKUP(D34,products!$A$2:$P$16,4,0)</f>
@@ -4732,15 +4732,15 @@
       </c>
       <c r="O34" s="0" t="str">
         <f aca="false">VLOOKUP($D34,products!$A$2:$P$16,11,0)</f>
-        <v>Cat_2</v>
+        <v>Cat_1</v>
       </c>
       <c r="P34" s="0" t="n">
         <f aca="false">D34</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="Q34" s="0" t="str">
         <f aca="false">VLOOKUP($D34,products!$A$2:$P$16,13,0)</f>
-        <v>SubCat_21</v>
+        <v>SubCat_13</v>
       </c>
       <c r="R34" s="0" t="str">
         <f aca="false">VLOOKUP($D34,products!$A$2:$P$16,14,0)</f>
@@ -4760,24 +4760,24 @@
       </c>
       <c r="V34" s="0" t="str">
         <f aca="false">VLOOKUP($D34,products!$A$2:$P$16,9,0)</f>
-        <v>SubBrand_122</v>
+        <v>SubBrand_121</v>
       </c>
       <c r="W34" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X34" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Y34" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Z34" s="0" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
@@ -4786,10 +4786,10 @@
         <v>5</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>5</v>
@@ -4802,11 +4802,11 @@
       </c>
       <c r="I35" s="0" t="str">
         <f aca="false">VLOOKUP(D35,products!$A$2:$P$16,2,0)</f>
-        <v>Product_122_22_09</v>
+        <v>Product_122_21_08</v>
       </c>
       <c r="J35" s="0" t="str">
         <f aca="false">VLOOKUP(D35,products!$A$2:$P$16,3,0)</f>
-        <v>122_22_09</v>
+        <v>122_21_08</v>
       </c>
       <c r="K35" s="0" t="str">
         <f aca="false">VLOOKUP(D35,products!$A$2:$P$16,4,0)</f>
@@ -4830,11 +4830,11 @@
       </c>
       <c r="P35" s="0" t="n">
         <f aca="false">D35</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q35" s="0" t="str">
         <f aca="false">VLOOKUP($D35,products!$A$2:$P$16,13,0)</f>
-        <v>SubCat_22</v>
+        <v>SubCat_21</v>
       </c>
       <c r="R35" s="0" t="str">
         <f aca="false">VLOOKUP($D35,products!$A$2:$P$16,14,0)</f>
@@ -4869,22 +4869,102 @@
         <v>67</v>
       </c>
     </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="I36" s="0" t="str">
+        <f aca="false">VLOOKUP(D36,products!$A$2:$P$16,2,0)</f>
+        <v>Product_122_22_09</v>
+      </c>
+      <c r="J36" s="0" t="str">
+        <f aca="false">VLOOKUP(D36,products!$A$2:$P$16,3,0)</f>
+        <v>122_22_09</v>
+      </c>
+      <c r="K36" s="0" t="str">
+        <f aca="false">VLOOKUP(D36,products!$A$2:$P$16,4,0)</f>
+        <v>SKU</v>
+      </c>
+      <c r="L36" s="0" t="str">
+        <f aca="false">VLOOKUP($D36,products!$A$2:$P$16,8,0)</f>
+        <v>Brand_12</v>
+      </c>
+      <c r="M36" s="0" t="str">
+        <f aca="false">VLOOKUP($D36,products!$A$2:$P$16,6,0)</f>
+        <v>TCCC</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <f aca="false">VLOOKUP($D36,products!$A$2:$P$16,10,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O36" s="0" t="str">
+        <f aca="false">VLOOKUP($D36,products!$A$2:$P$16,11,0)</f>
+        <v>Cat_2</v>
+      </c>
+      <c r="P36" s="0" t="n">
+        <f aca="false">D36</f>
+        <v>9</v>
+      </c>
+      <c r="Q36" s="0" t="str">
+        <f aca="false">VLOOKUP($D36,products!$A$2:$P$16,13,0)</f>
+        <v>SubCat_22</v>
+      </c>
+      <c r="R36" s="0" t="str">
+        <f aca="false">VLOOKUP($D36,products!$A$2:$P$16,14,0)</f>
+        <v>FF_1</v>
+      </c>
+      <c r="S36" s="0" t="n">
+        <f aca="false">VLOOKUP($D36,products!$A$2:$P$16,15,0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="T36" s="0" t="str">
+        <f aca="false">VLOOKUP($D36,products!$A$2:$P$16,16,0)</f>
+        <v>l</v>
+      </c>
+      <c r="U36" s="0" t="str">
+        <f aca="false">VLOOKUP($D36,products!$A$2:$P$16,8,0)</f>
+        <v>Brand_12</v>
+      </c>
+      <c r="V36" s="0" t="str">
+        <f aca="false">VLOOKUP($D36,products!$A$2:$P$16,9,0)</f>
+        <v>SubBrand_122</v>
+      </c>
+      <c r="W36" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="X36" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y36" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z36" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Z35">
-    <filterColumn colId="14">
-      <filters>
-        <filter val="Cat_2"/>
-        <filter val="Cat_1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="22">
-      <filters>
-        <filter val="Scene_type_3"/>
-        <filter val="Scene_type_2"/>
-        <filter val="Scene_type_1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Z36"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
kpi function tests added
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Tests/Data/test_case_data.xlsx
+++ b/Projects/CCRU/Tests/Data/test_case_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,6 +21,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">scif!$A$1:$Z$36</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">scif!$A$1:$Z$36</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">scif!$A$1:$Z$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">scif!$A$1:$Z$36</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -289,13 +290,13 @@
     <t xml:space="preserve">facings</t>
   </si>
   <si>
+    <t xml:space="preserve">1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.5</t>
   </si>
   <si>
     <t xml:space="preserve">0.5</t>
@@ -436,23 +437,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9676113360324"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1376518218623"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.251012145749"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6558704453441"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.8825910931174"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.251012145749"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.5384615384615"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.9109311740891"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.2550607287449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.9676113360324"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="5.82591093117409"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.6558704453441"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9676113360324"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6234817813765"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.6801619433198"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3967611336032"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6234817813765"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.080971659919"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4534412955466"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.0242914979757"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6801619433198"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9109311740891"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.3967611336032"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.5101214574899"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.1093117408907"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.17004048582996"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.4534412955466"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1289,16 +1290,16 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5384615384615"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="27.6518218623482"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2550607287449"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6801619433198"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="29.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5101214574899"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1404,16 +1405,16 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6558704453441"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5384615384615"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0242914979757"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4534412955466"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6801619433198"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9392712550607"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1443,7 +1444,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>72</v>
@@ -1465,7 +1466,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>74</v>
@@ -1476,7 +1477,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>75</v>
@@ -1506,9 +1507,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0526315789474"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1561,36 +1562,36 @@
   </sheetPr>
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q13" activeCellId="0" sqref="Q13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.22672064777328"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3684210526316"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3117408906883"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.71255060728745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6558704453441"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5384615384615"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.0242914979757"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.1376518218623"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.9676113360324"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.8825910931174"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.251012145749"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5384615384615"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0526315789474"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.2550607287449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.9676113360324"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="5.82591093117409"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="11.6558704453441"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="21.251012145749"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="27.6518218623482"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.2550607287449"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.45748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1133603238866"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4534412955466"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.6801619433198"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9392712550607"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.6234817813765"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.6801619433198"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.3967611336032"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.0242914979757"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="27.080971659919"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.6801619433198"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9109311740891"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.9676113360324"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.5101214574899"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.1093117408907"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.17004048582996"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="12.4534412955466"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.251012145749"/>
+    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="29.7085020242915"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.5101214574899"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
KPI score calculation precision
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Tests/Data/test_case_data.xlsx
+++ b/Projects/CCRU/Tests/Data/test_case_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,6 +30,8 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$Z$36</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$Z$36</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$Z$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$Z$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$Z$36</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -748,7 +750,7 @@
   </si>
   <si>
     <t xml:space="preserve">INSERT INTO report.kpi_level_2_results (parent_fk, numerator_id, denominator_id, weight, kpi_level_2_fk, session_fk, denominator_result_after_actions, numerator_result_after_actions, numerator_result, result, denominator_result, context_id, score_after_actions, score, target, kpi_level_2_target_fk)
-           VALUES (NULL, '1', '1', '1', '1', '1', NULL, '0', '2.0', '66.67', '3.0', NULL, '0', '66.67', '100', NULL)</t>
+           VALUES (NULL, '1', '1', '1', '1', '1', NULL, '0', '2.0', '66.667', '3.0', NULL, '0', '66.667', '100', NULL)</t>
   </si>
 </sst>
 </file>
@@ -876,27 +878,28 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="2" sqref="D2:D24 E2:E25 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5101214574899"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1093117408907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.7368421052632"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7368421052632"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.1093117408907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.1376518218623"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.336032388664"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.6801619433198"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.8825910931174"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.7651821862348"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.9676113360324"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.8825910931174"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.65587044534413"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3684210526316"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.336032388664"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.6477732793522"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.2793522267206"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.336032388664"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.9635627530364"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8259109311741"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.336032388664"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.6801619433198"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.7651821862348"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.9919028340081"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.5101214574899"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.9676113360324"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.79757085020243"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.8259109311741"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,13 +1735,13 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="2" sqref="D2:D24 E2:E25 E1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="135.627530364372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2212,15 +2215,16 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="2" sqref="D2:D24 E2:E25 C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6801619433198"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="36.9068825910931"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9676113360324"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7651821862348"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.3927125506073"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="42.6194331983806"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5101214574899"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2327,14 +2331,15 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="2" sqref="D2:D24 E2:E25 C10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6801619433198"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8259109311741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7651821862348"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7651821862348"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2422,13 +2427,14 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="2" sqref="D2:D24 E2:E25 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.3076923076923"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.9068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5344129554656"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4777327935223"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2482,34 +2488,35 @@
   <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="2" sqref="D2:D24 E2:E25 H12"/>
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.25506072874494"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8259109311741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8542510121458"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="12.9109311740891"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6801619433198"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.1093117408907"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.7368421052632"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.7368421052632"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.1376518218623"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="33.7085020242915"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.6801619433198"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.8825910931174"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.5101214574899"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="22.9676113360324"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.8825910931174"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="7.65587044534413"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="28.336032388664"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="26.2793522267206"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="36.9068825910931"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.9676113360324"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.94331983805668"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="14.7408906882591"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8259109311741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.7651821862348"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7651821862348"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.336032388664"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="35.6477732793522"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.2793522267206"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.336032388664"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="38.9635627530364"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.7651821862348"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.3684210526316"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="26.5101214574899"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.9676113360324"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.79757085020243"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="17.8259109311741"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="32.6801619433198"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="30.3927125506073"/>
+    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="42.6194331983806"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="26.5101214574899"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5903,35 +5910,34 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D2:D24 E2:E25"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.54251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7408906882591"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5951417004049"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0242914979757"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9392712550607"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.79757085020243"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8825910931174"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.9392712550607"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6234817813765"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.080971659919"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.6558704453441"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="12.9109311740891"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.0242914979757"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.9068825910931"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.1943319838057"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.5951417004049"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="23.4251012145749"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="21.9392712550607"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.6518218623482"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.6558704453441"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.5384615384615"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0242914979757"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.2226720647773"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8542510121458"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.995951417004"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.93927125506073"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.9676113360324"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.251012145749"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.4817813765182"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.0526315789474"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3684210526316"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.1417004048583"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="14.7408906882591"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.6518218623482"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="28.7935222672065"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="22.165991902834"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.2226720647773"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.8218623481781"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="26.9635627530364"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="25.251012145749"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="22.6234817813765"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="13.3684210526316"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.9392712550607"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6274,15 +6280,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="D2:D24 E2:E25 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3967611336032"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.080971659919"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3967611336032"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6348,15 +6352,13 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D2:D24 E2:E25"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3967611336032"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.080971659919"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.9392712550607"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6654,14 +6656,12 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="D2:D24 E2:E25 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3967611336032"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.9392712550607"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6801619433198"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>